<commit_message>
Update npm dependencies and fix import in Role module
</commit_message>
<xml_diff>
--- a/hcmue/static/resources/template_2a.xlsx
+++ b/hcmue/static/resources/template_2a.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lekhp\Desktop\work\hcmue-rlsv-api\hcmue\static\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lkphuong/Desktop/vtcode_never_die/hcmue-rlsv-api/hcmue/static/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E24CCFB4-1FBA-4566-B82E-EA3D809DD35D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08C2AFC7-899A-7A4B-A666-76F048B69619}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{6AA4FCD2-BD11-441E-B767-FFD25C4AC7D8}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18040" xr2:uid="{6AA4FCD2-BD11-441E-B767-FFD25C4AC7D8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
   <si>
     <t>TRƯỜNG ĐẠI HỌC SƯ PHẠM</t>
   </si>
@@ -150,6 +150,9 @@
   </si>
   <si>
     <t>CHỦ TỊCH HĐRL KHOA</t>
+  </si>
+  <si>
+    <t>Cố vấn học tập</t>
   </si>
 </sst>
 </file>
@@ -219,7 +222,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -242,11 +245,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -261,31 +290,37 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -419,9 +454,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -459,7 +494,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -565,7 +600,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -707,7 +742,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -715,95 +750,100 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DCD1B7B-1F09-4C5B-83CC-0AC76441C9F5}">
-  <dimension ref="A1:K19"/>
+  <dimension ref="A1:L19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B12" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="4" max="4" width="12.85546875" customWidth="1"/>
-    <col min="5" max="5" width="15.42578125" customWidth="1"/>
-    <col min="11" max="11" width="15.42578125" customWidth="1"/>
+    <col min="4" max="4" width="12.83203125" customWidth="1"/>
+    <col min="5" max="5" width="15.5" customWidth="1"/>
+    <col min="11" max="11" width="17.33203125" customWidth="1"/>
+    <col min="12" max="12" width="15.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.15">
       <c r="J1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
+    <row r="3" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="13"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="F3" s="12" t="s">
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="F3" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="12"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="12"/>
-      <c r="J3" s="12"/>
-      <c r="K3" s="12"/>
-    </row>
-    <row r="4" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A4" s="13" t="s">
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="8"/>
+    </row>
+    <row r="4" spans="1:12" ht="18" x14ac:dyDescent="0.2">
+      <c r="A4" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="13"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="F4" s="8" t="s">
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="F4" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="8"/>
-      <c r="K4" s="8"/>
-    </row>
-    <row r="5" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="12" t="s">
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="10"/>
+      <c r="L4" s="10"/>
+    </row>
+    <row r="5" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="12"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
-    </row>
-    <row r="7" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A7" s="8" t="s">
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+    </row>
+    <row r="7" spans="1:12" ht="18" x14ac:dyDescent="0.2">
+      <c r="A7" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="8"/>
-      <c r="K7" s="8"/>
-    </row>
-    <row r="8" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A8" s="8" t="s">
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="10"/>
+      <c r="K7" s="10"/>
+      <c r="L7" s="10"/>
+    </row>
+    <row r="8" spans="1:12" ht="18" x14ac:dyDescent="0.2">
+      <c r="A8" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="8"/>
-      <c r="J8" s="8"/>
-      <c r="K8" s="8"/>
-    </row>
-    <row r="9" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10"/>
+      <c r="K8" s="10"/>
+      <c r="L8" s="10"/>
+    </row>
+    <row r="9" spans="1:12" ht="18" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -815,58 +855,63 @@
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
-    </row>
-    <row r="10" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="11" t="s">
+      <c r="L9" s="1"/>
+    </row>
+    <row r="10" spans="1:12" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="11" t="s">
+      <c r="D10" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="11" t="s">
+      <c r="E10" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="F10" s="11" t="s">
+      <c r="F10" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="G10" s="11" t="s">
+      <c r="G10" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="H10" s="11" t="s">
+      <c r="H10" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="I10" s="11" t="s">
+      <c r="I10" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="J10" s="11"/>
-      <c r="K10" s="11" t="s">
+      <c r="J10" s="7"/>
+      <c r="K10" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="L10" s="7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="11"/>
-      <c r="B11" s="11"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="11"/>
+    <row r="11" spans="1:12" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="7"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
       <c r="I11" s="3" t="s">
         <v>24</v>
       </c>
       <c r="J11" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="K11" s="11"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K11" s="16"/>
+      <c r="L11" s="7"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A12" s="5"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
@@ -878,17 +923,18 @@
       <c r="I12" s="5"/>
       <c r="J12" s="5"/>
       <c r="K12" s="5"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C13" s="9" t="s">
+      <c r="L12" s="5"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="C13" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="D13" s="9"/>
+      <c r="D13" s="13"/>
       <c r="E13" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" ht="17" x14ac:dyDescent="0.15">
       <c r="D14" s="4" t="s">
         <v>7</v>
       </c>
@@ -898,79 +944,83 @@
       <c r="F14" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G14" s="14"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G14" s="6"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.15">
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
       <c r="G15" s="5"/>
     </row>
-    <row r="16" spans="1:11" ht="114" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="10" t="s">
+    <row r="16" spans="1:12" ht="114" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="B16" s="10"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="10"/>
-      <c r="G16" s="10"/>
-      <c r="H16" s="10"/>
-      <c r="I16" s="10"/>
-      <c r="J16" s="10"/>
-      <c r="K16" s="10"/>
-    </row>
-    <row r="18" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="G18" s="6" t="s">
+      <c r="B16" s="14"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="14"/>
+      <c r="I16" s="14"/>
+      <c r="J16" s="14"/>
+      <c r="K16" s="14"/>
+      <c r="L16" s="14"/>
+    </row>
+    <row r="18" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="G18" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="H18" s="6"/>
-      <c r="I18" s="6"/>
-      <c r="J18" s="6"/>
-      <c r="K18" s="6"/>
-    </row>
-    <row r="19" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="7" t="s">
+      <c r="H18" s="11"/>
+      <c r="I18" s="11"/>
+      <c r="J18" s="11"/>
+      <c r="K18" s="11"/>
+      <c r="L18" s="11"/>
+    </row>
+    <row r="19" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A19" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
+      <c r="B19" s="12"/>
+      <c r="C19" s="12"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
-      <c r="F19" s="7" t="s">
+      <c r="F19" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="G19" s="7"/>
-      <c r="H19" s="7"/>
-      <c r="I19" s="7"/>
-      <c r="J19" s="7"/>
-      <c r="K19" s="7"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="12"/>
+      <c r="I19" s="12"/>
+      <c r="J19" s="12"/>
+      <c r="K19" s="12"/>
+      <c r="L19" s="12"/>
     </row>
   </sheetData>
-  <mergeCells count="22">
-    <mergeCell ref="H10:H11"/>
-    <mergeCell ref="A5:D5"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="F3:K3"/>
-    <mergeCell ref="F4:K4"/>
-    <mergeCell ref="A8:K8"/>
-    <mergeCell ref="G18:K18"/>
+  <mergeCells count="23">
+    <mergeCell ref="G18:L18"/>
     <mergeCell ref="A19:C19"/>
-    <mergeCell ref="A7:K7"/>
+    <mergeCell ref="A7:L7"/>
     <mergeCell ref="C13:D13"/>
-    <mergeCell ref="A16:K16"/>
+    <mergeCell ref="A16:L16"/>
     <mergeCell ref="B10:B11"/>
     <mergeCell ref="C10:C11"/>
     <mergeCell ref="D10:D11"/>
     <mergeCell ref="E10:E11"/>
     <mergeCell ref="A10:A11"/>
     <mergeCell ref="I10:J10"/>
-    <mergeCell ref="K10:K11"/>
-    <mergeCell ref="F19:K19"/>
+    <mergeCell ref="L10:L11"/>
+    <mergeCell ref="F19:L19"/>
     <mergeCell ref="F10:F11"/>
     <mergeCell ref="G10:G11"/>
+    <mergeCell ref="K10:K11"/>
+    <mergeCell ref="H10:H11"/>
+    <mergeCell ref="A5:D5"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="F3:L3"/>
+    <mergeCell ref="F4:L4"/>
+    <mergeCell ref="A8:L8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>